<commit_message>
Other scripts and data
</commit_message>
<xml_diff>
--- a/06_processed_data/carcasses/3_hy.clan.members.xlsx
+++ b/06_processed_data/carcasses/3_hy.clan.members.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hyena_roadkill_project\06_processed_data\carcasses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F793EEF8-7D30-4E91-8F7E-ADFF35C5A285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A49F3B-489C-40EF-BB2B-3D7C06CC324E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3576" yWindow="3036" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3_hy.clan.members" sheetId="1" r:id="rId1"/>
@@ -127,9 +127,6 @@
     <t>0.5</t>
   </si>
   <si>
-    <t>Hy_051</t>
-  </si>
-  <si>
     <t>Z142</t>
   </si>
   <si>
@@ -292,9 +289,6 @@
     <t>no records for 2020</t>
   </si>
   <si>
-    <t>Hy_089</t>
-  </si>
-  <si>
     <t>Z196</t>
   </si>
   <si>
@@ -304,37 +298,43 @@
     <t>0.42</t>
   </si>
   <si>
-    <t>Hy_060</t>
-  </si>
-  <si>
-    <t>Hy_035</t>
-  </si>
-  <si>
-    <t>Hy_050</t>
-  </si>
-  <si>
-    <t>Hy_055</t>
-  </si>
-  <si>
-    <t>Hy_062</t>
-  </si>
-  <si>
-    <t>Hy_064</t>
-  </si>
-  <si>
-    <t>Hy_066</t>
-  </si>
-  <si>
     <t>Hy_071</t>
   </si>
   <si>
-    <t>Hy_074</t>
-  </si>
-  <si>
     <t>Hy_083</t>
   </si>
   <si>
-    <t>Hy_088</t>
+    <t>Hy_032</t>
+  </si>
+  <si>
+    <t>Hy_047</t>
+  </si>
+  <si>
+    <t>Hy_048</t>
+  </si>
+  <si>
+    <t>Hy_052</t>
+  </si>
+  <si>
+    <t>Hy_056</t>
+  </si>
+  <si>
+    <t>Hy_059</t>
+  </si>
+  <si>
+    <t>Hy_063</t>
+  </si>
+  <si>
+    <t>Hy_061</t>
+  </si>
+  <si>
+    <t>Hy_068</t>
+  </si>
+  <si>
+    <t>Hy_080</t>
+  </si>
+  <si>
+    <t>Hy_084</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1180,7 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1243,37 +1243,37 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="F2" s="1">
-        <v>37475</v>
+        <v>43489</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
-        <v>24</v>
+      <c r="I2">
+        <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -1288,27 +1288,27 @@
         <v>24</v>
       </c>
       <c r="R2" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="F3" s="1">
-        <v>40653</v>
+        <v>42157</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
@@ -1317,10 +1317,10 @@
         <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="K3" t="s">
         <v>33</v>
@@ -1328,70 +1328,61 @@
       <c r="L3">
         <v>1</v>
       </c>
-      <c r="M3" t="s">
-        <v>34</v>
+      <c r="M3">
+        <v>1</v>
       </c>
       <c r="N3">
-        <v>697640</v>
+        <v>696378</v>
       </c>
       <c r="O3">
-        <v>9730619</v>
+        <v>9731342</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F4" s="1">
-        <v>40803</v>
+        <v>42558</v>
       </c>
       <c r="G4" t="s">
         <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="I4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" t="s">
         <v>41</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>42</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
         <v>43</v>
       </c>
-      <c r="L4" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4">
-        <v>708643</v>
-      </c>
-      <c r="O4">
-        <v>9727427</v>
-      </c>
-      <c r="P4">
-        <v>708726</v>
-      </c>
-      <c r="Q4">
-        <v>9727641</v>
-      </c>
-      <c r="R4" t="s">
-        <v>45</v>
+      <c r="N4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -1399,16 +1390,16 @@
         <v>97</v>
       </c>
       <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>47</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>48</v>
-      </c>
-      <c r="E5" t="s">
-        <v>49</v>
       </c>
       <c r="F5" s="1">
         <v>41317</v>
@@ -1420,13 +1411,13 @@
         <v>23</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" t="s">
         <v>42</v>
-      </c>
-      <c r="K5" t="s">
-        <v>43</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -1443,84 +1434,90 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="F6" s="1">
-        <v>41659</v>
+        <v>40803</v>
       </c>
       <c r="G6" t="s">
         <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="J6" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="K6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="L6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" t="s">
+        <v>34</v>
       </c>
       <c r="N6">
-        <v>697280</v>
+        <v>708643</v>
       </c>
       <c r="O6">
-        <v>9726969</v>
+        <v>9727427</v>
+      </c>
+      <c r="P6">
+        <v>708726</v>
+      </c>
+      <c r="Q6">
+        <v>9727641</v>
       </c>
       <c r="R6" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1">
-        <v>42043</v>
+        <v>40653</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="H7" t="s">
         <v>23</v>
       </c>
       <c r="I7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="J7" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="K7" t="s">
         <v>33</v>
@@ -1528,28 +1525,34 @@
       <c r="L7">
         <v>1</v>
       </c>
-      <c r="M7">
-        <v>1</v>
+      <c r="M7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7">
+        <v>697640</v>
+      </c>
+      <c r="O7">
+        <v>9730619</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="F8" s="1">
-        <v>42157</v>
+        <v>43877</v>
       </c>
       <c r="G8" t="s">
         <v>30</v>
@@ -1558,60 +1561,63 @@
         <v>23</v>
       </c>
       <c r="I8" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="J8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" t="s">
         <v>42</v>
       </c>
-      <c r="K8" t="s">
-        <v>33</v>
-      </c>
       <c r="L8">
         <v>1</v>
       </c>
       <c r="M8">
         <v>1</v>
       </c>
-      <c r="N8">
-        <v>696378</v>
-      </c>
-      <c r="O8">
-        <v>9731342</v>
+      <c r="N8" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" t="s">
+        <v>24</v>
+      </c>
+      <c r="R8" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="F9" s="1">
-        <v>42220</v>
+        <v>43877</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="H9" t="s">
         <v>23</v>
       </c>
       <c r="I9" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="J9" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="K9" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -1619,49 +1625,46 @@
       <c r="M9">
         <v>1</v>
       </c>
-      <c r="N9">
-        <v>697788</v>
-      </c>
-      <c r="O9">
-        <v>9727760</v>
-      </c>
-      <c r="P9">
-        <v>696990</v>
-      </c>
-      <c r="Q9">
-        <v>9731202</v>
+      <c r="N9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" t="s">
+        <v>24</v>
+      </c>
+      <c r="R9" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="F10" s="1">
-        <v>42528</v>
+        <v>41659</v>
       </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="H10" t="s">
         <v>23</v>
       </c>
       <c r="I10" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="J10" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="K10" t="s">
         <v>22</v>
@@ -1672,90 +1675,96 @@
       <c r="M10">
         <v>1</v>
       </c>
-      <c r="N10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O10" t="s">
-        <v>24</v>
+      <c r="N10">
+        <v>697280</v>
+      </c>
+      <c r="O10">
+        <v>9726969</v>
+      </c>
+      <c r="R10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="F11" s="1">
-        <v>42558</v>
+        <v>37475</v>
       </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H11" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="I11" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="J11" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="K11" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="L11">
         <v>1</v>
       </c>
-      <c r="M11" t="s">
-        <v>44</v>
+      <c r="M11">
+        <v>1</v>
       </c>
       <c r="N11" t="s">
         <v>24</v>
       </c>
       <c r="O11" t="s">
         <v>24</v>
+      </c>
+      <c r="R11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="F12" s="1">
-        <v>43489</v>
+        <v>42043</v>
       </c>
       <c r="G12" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H12" t="s">
         <v>23</v>
       </c>
-      <c r="I12">
-        <v>1</v>
+      <c r="I12" t="s">
+        <v>24</v>
       </c>
       <c r="J12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="K12" t="s">
         <v>33</v>
@@ -1765,50 +1774,41 @@
       </c>
       <c r="M12">
         <v>1</v>
-      </c>
-      <c r="N12" t="s">
-        <v>24</v>
-      </c>
-      <c r="O12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R12" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="F13" s="1">
-        <v>43877</v>
+        <v>42220</v>
       </c>
       <c r="G13" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H13" t="s">
         <v>23</v>
       </c>
       <c r="I13" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="J13" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="K13" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="L13">
         <v>1</v>
@@ -1816,49 +1816,52 @@
       <c r="M13">
         <v>1</v>
       </c>
-      <c r="N13" t="s">
-        <v>24</v>
-      </c>
-      <c r="O13" t="s">
-        <v>24</v>
-      </c>
-      <c r="R13" t="s">
-        <v>89</v>
+      <c r="N13">
+        <v>697788</v>
+      </c>
+      <c r="O13">
+        <v>9727760</v>
+      </c>
+      <c r="P13">
+        <v>696990</v>
+      </c>
+      <c r="Q13">
+        <v>9731202</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="F14" s="1">
-        <v>43877</v>
+        <v>42528</v>
       </c>
       <c r="G14" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H14" t="s">
         <v>23</v>
       </c>
       <c r="I14" t="s">
-        <v>88</v>
+        <v>24</v>
       </c>
       <c r="J14" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="K14" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="L14">
         <v>1</v>
@@ -1871,17 +1874,14 @@
       </c>
       <c r="O14" t="s">
         <v>24</v>
-      </c>
-      <c r="R14" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R17">
-    <sortCondition ref="F2:F17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R16">
+    <sortCondition ref="I2:I16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>